<commit_message>
UI Test cases 2 and 3 are completed
</commit_message>
<xml_diff>
--- a/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
+++ b/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Log\GitRepo\internetherokuapp\SourceCode\CSharpSolution\Framework\HerokuAppAutomation\UI.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054AFE9E-453F-4DEB-926C-32CA618BF9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4209496-D539-4912-B06E-D4AB0E62D9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UISuite" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Example 2: Element rendered after the fact</t>
   </si>
   <si>
-    <t>Start Button Text</t>
-  </si>
-  <si>
     <t>Start</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>After Loading Message</t>
   </si>
   <si>
-    <t>TC2_DynamicLoading</t>
-  </si>
-  <si>
     <t>Valid Username Obtained from Portal</t>
   </si>
   <si>
@@ -98,6 +92,21 @@
   </si>
   <si>
     <t>Test Case 1 - Form Authentication Demonstration</t>
+  </si>
+  <si>
+    <t>Test Case 2 - Dynamic Loading Demonstration</t>
+  </si>
+  <si>
+    <t>Button Text</t>
+  </si>
+  <si>
+    <t>Click Link Text</t>
+  </si>
+  <si>
+    <t>Click Here</t>
+  </si>
+  <si>
+    <t>Test Case 3 - Multiple Windows Demonstration</t>
   </si>
 </sst>
 </file>
@@ -128,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +147,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -188,6 +209,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -473,7 +506,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -500,148 +533,154 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="D9" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">

</xml_diff>

<commit_message>
API Automation Test Case 1 added
</commit_message>
<xml_diff>
--- a/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
+++ b/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Log\GitRepo\internetherokuapp\SourceCode\CSharpSolution\Framework\HerokuAppAutomation\UI.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4209496-D539-4912-B06E-D4AB0E62D9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92D8D8E-69AA-47A9-9A58-7C66D8E88C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UISuite" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -107,13 +107,41 @@
   </si>
   <si>
     <t>Test Case 3 - Multiple Windows Demonstration</t>
+  </si>
+  <si>
+    <t>uri</t>
+  </si>
+  <si>
+    <t>/booking</t>
+  </si>
+  <si>
+    <t>Test Case 1 - Create Booking Postive scenario</t>
+  </si>
+  <si>
+    <t>Request Body</t>
+  </si>
+  <si>
+    <t>{
+    "bookingid": 25,
+    "booking": {
+        "firstname": "Jim",
+        "lastname": "Brown",
+        "totalprice": 111,
+        "depositpaid": true,
+        "bookingdates": {
+            "checkin": "2018-01-01",
+            "checkout": "2019-01-01"
+        },
+        "additionalneeds": "Breakfast"
+    }
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +160,13 @@
       <b/>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -222,6 +257,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -789,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9087AB3-733F-428C-B4A0-666075F2F7F6}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -820,17 +864,29 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="180" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
@@ -1020,5 +1076,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed Unnecessary class files and test data changes for API
</commit_message>
<xml_diff>
--- a/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
+++ b/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Log\GitRepo\internetherokuapp\SourceCode\CSharpSolution\Framework\HerokuAppAutomation\UI.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92D8D8E-69AA-47A9-9A58-7C66D8E88C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64C14AC-E492-4E47-969C-1A7270463120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -834,7 +834,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Removed TestApp, Test Data update, Few Project structure changes, TestExecutor renamed to TestInitializer
</commit_message>
<xml_diff>
--- a/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
+++ b/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Log\GitRepo\internetherokuapp\SourceCode\CSharpSolution\Framework\HerokuAppAutomation\UI.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64C14AC-E492-4E47-969C-1A7270463120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC9098D-F2FE-4C09-ACFE-7195308D5CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UISuite" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -122,19 +122,60 @@
   </si>
   <si>
     <t>{
-    "bookingid": 25,
-    "booking": {
-        "firstname": "Jim",
-        "lastname": "Brown",
-        "totalprice": 111,
-        "depositpaid": true,
-        "bookingdates": {
-            "checkin": "2018-01-01",
-            "checkout": "2019-01-01"
-        },
-        "additionalneeds": "Breakfast"
-    }
+    "firstname" : "Jim",
+    "lastname" : "Brown",
+    "totalprice" : 111,
+    "depositpaid" : true,
+    "bookingdates" : {
+        "checkin" : "2018-01-01",
+        "checkout" : "2019-01-01"
+    },
+    "additionalneeds" : "Breakfast"
 }</t>
+  </si>
+  <si>
+    <t>Expected Response Code</t>
+  </si>
+  <si>
+    <t>Booking ID Created</t>
+  </si>
+  <si>
+    <t>Test Case 2 - Create Booking Negative scenario Null Check</t>
+  </si>
+  <si>
+    <t>Test Case 3 - Create Booking Negative scenario Invalid Date Check</t>
+  </si>
+  <si>
+    <t>{
+    "firstname" : null,
+    "lastname" : null,
+    "totalprice" : null,
+    "depositpaid" : null,
+    "bookingdates" : {
+        "checkin" : null,
+        "checkout" : null
+    },
+    "additionalneeds" : null
+}</t>
+  </si>
+  <si>
+    <t>{
+    "firstname" : "Jim",
+    "lastname" : "Brown",
+    "totalprice" : 12,
+    "depositpaid" : false,
+    "bookingdates" : {
+        "checkin" : "2021-13-31",
+        "checkout" : "2021-13-32"
+    },
+    "additionalneeds" : null
+}</t>
+  </si>
+  <si>
+    <t>Expected Response Message</t>
+  </si>
+  <si>
+    <t>Invalid date</t>
   </si>
 </sst>
 </file>
@@ -172,7 +213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +235,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -258,14 +305,23 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,16 +887,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9087AB3-733F-428C-B4A0-666075F2F7F6}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="4" customWidth="1"/>
-    <col min="2" max="2" width="56.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="1"/>
@@ -861,21 +917,21 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="180" x14ac:dyDescent="0.3">
-      <c r="A3" s="14">
+    <row r="3" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -889,79 +945,131 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="11">
+        <v>200</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="B6" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="B7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="B8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="9">
+        <v>500</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="B9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="140.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="12">
+        <v>200</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="B12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="17">
         <v>12</v>
       </c>
       <c r="B13" s="6"/>
@@ -969,7 +1077,7 @@
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14" s="17">
         <v>13</v>
       </c>
       <c r="B14" s="6"/>
@@ -977,7 +1085,7 @@
       <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15" s="17">
         <v>14</v>
       </c>
       <c r="B15" s="6"/>
@@ -985,13 +1093,17 @@
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
+      <c r="A16" s="17">
+        <v>15</v>
+      </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
+      <c r="A17" s="17">
+        <v>16</v>
+      </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1074,6 +1186,18 @@
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
API Testcase 4 completed
</commit_message>
<xml_diff>
--- a/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
+++ b/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
@@ -8,25 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Log\GitRepo\internetherokuapp\SourceCode\CSharpSolution\Framework\HerokuAppAutomation\UI.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC9098D-F2FE-4C09-ACFE-7195308D5CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA98F48-4A2D-4E39-91C6-B7A1CF13C410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UISuite" sheetId="1" r:id="rId1"/>
     <sheet name="APISuite" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -172,10 +181,45 @@
 }</t>
   </si>
   <si>
-    <t>Expected Response Message</t>
-  </si>
-  <si>
     <t>Invalid date</t>
+  </si>
+  <si>
+    <t>Test Case 4 - Get Booking Postive scenario</t>
+  </si>
+  <si>
+    <t>Valid Booking ID</t>
+  </si>
+  <si>
+    <t>Expected Response Body</t>
+  </si>
+  <si>
+    <t>{
+    "bookingid": @@@,
+    "booking": {
+        "firstname": "Jim",
+        "lastname": "Brown",
+        "totalprice": 111,
+        "depositpaid": true,
+        "bookingdates": {
+            "checkin": "2018-01-01",
+            "checkout": "2019-01-01"
+        },
+        "additionalneeds": "Breakfast"
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "firstname": "Jim",
+    "lastname": "Brown",
+    "totalprice": 111,
+    "depositpaid": true,
+    "bookingdates": {
+        "checkin": "2018-01-01",
+        "checkout": "2019-01-01"
+    },
+    "additionalneeds": "Breakfast"
+}</t>
   </si>
 </sst>
 </file>
@@ -213,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,12 +279,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -320,8 +358,29 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,17 +946,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9087AB3-733F-428C-B4A0-666075F2F7F6}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" style="4" customWidth="1"/>
-    <col min="2" max="2" width="75.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="21" customWidth="1"/>
+    <col min="2" max="2" width="75.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" style="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="1"/>
   </cols>
@@ -917,13 +976,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="11" t="s">
@@ -931,7 +990,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -945,258 +1004,319 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="17">
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="11">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+    <row r="5" spans="1:4" ht="262.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+        <v>27</v>
+      </c>
+      <c r="D7" s="9" t="str">
+        <f>D2</f>
+        <v>/booking</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
+        <v>8</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D9" s="9">
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
-        <v>8</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="140.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
         <v>9</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
-        <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="12">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="D11" s="11" t="str">
+        <f>D2</f>
+        <v>/booking</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="140.25" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
+        <v>10</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>39</v>
+      <c r="C12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="12">
+        <v>200</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
+        <v>12</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="9" t="str">
+        <f>D2&amp;"/{0}"</f>
+        <v>/booking/{0}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="18">
         <v>13</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
+      <c r="B16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="206.25" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="17">
+      <c r="B18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="A21" s="17">
+        <v>17</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
       <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="20"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="20"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="20"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="20"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
API Test cases committed
</commit_message>
<xml_diff>
--- a/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
+++ b/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Log\GitRepo\internetherokuapp\SourceCode\CSharpSolution\Framework\HerokuAppAutomation\UI.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA98F48-4A2D-4E39-91C6-B7A1CF13C410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A457AB46-9DBC-4F1D-A6DF-597CADE69588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UISuite" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>/booking</t>
-  </si>
-  <si>
-    <t>Test Case 1 - Create Booking Postive scenario</t>
   </si>
   <si>
     <t>Request Body</t>
@@ -149,12 +146,6 @@
     <t>Booking ID Created</t>
   </si>
   <si>
-    <t>Test Case 2 - Create Booking Negative scenario Null Check</t>
-  </si>
-  <si>
-    <t>Test Case 3 - Create Booking Negative scenario Invalid Date Check</t>
-  </si>
-  <si>
     <t>{
     "firstname" : null,
     "lastname" : null,
@@ -182,9 +173,6 @@
   </si>
   <si>
     <t>Invalid date</t>
-  </si>
-  <si>
-    <t>Test Case 4 - Get Booking Postive scenario</t>
   </si>
   <si>
     <t>Valid Booking ID</t>
@@ -220,6 +208,96 @@
     },
     "additionalneeds": "Breakfast"
 }</t>
+  </si>
+  <si>
+    <t>Invalid Booking ID</t>
+  </si>
+  <si>
+    <t>Not Found</t>
+  </si>
+  <si>
+    <t>Auth Token</t>
+  </si>
+  <si>
+    <t>{
+    "firstname": "James",
+    "lastname": "Brown",
+    "totalprice": 111,
+    "depositpaid": true,
+    "bookingdates": {
+        "checkin": "2018-01-01",
+        "checkout": "2019-01-01"
+    },
+    "additionalneeds": "Breakfast"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "firstname" : "James",
+    "lastname" : "Brown",
+    "totalprice" : 111,
+    "depositpaid" : true,
+    "bookingdates" : {
+        "checkin" : "2018-13-31",
+        "checkout" : "2019-13-32"
+    },
+    "additionalneeds" : "Breakfast"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "firstname" : "James",
+    "lastname" : "Brown",
+    "totalprice" : 111,
+    "depositpaid" : true,
+    "bookingdates" : {
+        "checkin" : "2018-01-01",
+        "checkout" : "2019-01-01"
+    },
+    "additionalneeds" : "Breakfast"
+}</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Test Case 10 - Delete Booking Negative scenario with invalid Auth Token</t>
+  </si>
+  <si>
+    <t>Forbidden</t>
+  </si>
+  <si>
+    <t>InvalidAuthToken</t>
+  </si>
+  <si>
+    <t>Invalid Auth Token</t>
+  </si>
+  <si>
+    <t>Test Case 01 - Create Booking Postive scenario</t>
+  </si>
+  <si>
+    <t>Test Case 02 - Create Booking Negative scenario Null Check</t>
+  </si>
+  <si>
+    <t>Test Case 03 - Create Booking Negative scenario Invalid Date Check</t>
+  </si>
+  <si>
+    <t>Test Case 04 - Get Booking Postive scenario</t>
+  </si>
+  <si>
+    <t>Test Case 05 - Get Booking Negative scenario with invalid Booking ID</t>
+  </si>
+  <si>
+    <t>Test Case 06 - Update Booking Postive scenario</t>
+  </si>
+  <si>
+    <t>Test Case 07 - Update Booking Negative scenario with invalid Date</t>
+  </si>
+  <si>
+    <t>Test Case 08 - Delete Booking Postive scenario</t>
+  </si>
+  <si>
+    <t>Test Case 09 - Delete Booking Negative scenario with invalid Booking Id</t>
   </si>
 </sst>
 </file>
@@ -310,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -367,17 +445,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -946,17 +1018,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9087AB3-733F-428C-B4A0-666075F2F7F6}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" style="21" customWidth="1"/>
-    <col min="2" max="2" width="75.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="20" customWidth="1"/>
+    <col min="2" max="2" width="79.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="1"/>
   </cols>
@@ -980,7 +1052,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>27</v>
@@ -994,13 +1066,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1008,27 +1080,27 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="11">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="262.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="180" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1036,10 +1108,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="11"/>
     </row>
@@ -1048,7 +1120,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>27</v>
@@ -1063,13 +1135,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1077,31 +1149,33 @@
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="9">
         <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
+      <c r="A10" s="18">
+        <v>9</v>
+      </c>
       <c r="B10" s="14" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>27</v>
@@ -1113,27 +1187,27 @@
     </row>
     <row r="12" spans="1:4" ht="140.25" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="12">
         <v>200</v>
@@ -1141,182 +1215,496 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
+      <c r="A15" s="18">
+        <v>14</v>
+      </c>
       <c r="B15" s="14" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="9" t="str">
-        <f>D2&amp;"/{0}"</f>
+        <f>$D$2&amp;"/{0}"</f>
         <v>/booking/{0}</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
+      <c r="A17" s="18">
+        <v>16</v>
+      </c>
       <c r="B17" s="14" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="9">
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="206.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="17">
-        <v>14</v>
+    <row r="18" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
+        <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
-        <v>15</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="11" t="str">
+        <f>$D$2&amp;"/{0}"</f>
+        <v>/booking/{0}</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="17">
-        <v>16</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="11">
+        <v>1000000</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="17">
-        <v>17</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="11">
+        <v>404</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="17">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="6"/>
+      <c r="A23" s="18">
+        <v>22</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="9" t="str">
+        <f>$D$2&amp;"/{0}"</f>
+        <v>/booking/{0}</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="6"/>
+      <c r="A24" s="18">
+        <v>23</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="6"/>
+      <c r="A25" s="18">
+        <v>24</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="18">
+        <v>25</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="6"/>
+      <c r="A27" s="18">
+        <v>26</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="18">
+        <v>27</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="6"/>
+      <c r="A29" s="17">
+        <v>28</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="11" t="str">
+        <f>$D$2&amp;"/{0}"</f>
+        <v>/booking/{0}</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="17">
+        <v>29</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="6"/>
+      <c r="A31" s="17">
+        <v>30</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="17">
+        <v>31</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="20"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="6"/>
+      <c r="A33" s="17">
+        <v>32</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="11">
+        <v>200</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="20"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="6"/>
+      <c r="A34" s="17">
+        <v>33</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="6"/>
+      <c r="A35" s="18">
+        <v>34</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="9" t="str">
+        <f>$D$2&amp;"/{0}"</f>
+        <v>/booking/{0}</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="20"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="6"/>
+      <c r="A36" s="18">
+        <v>35</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="18">
+        <v>36</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="18">
+        <v>37</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="9">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="18">
+        <v>38</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="17">
+        <v>39</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="11" t="str">
+        <f>$D$2&amp;"/{0}"</f>
+        <v>/booking/{0}</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="17">
+        <v>40</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="17">
+        <v>41</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="11">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="17">
+        <v>42</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="11">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="17">
+        <v>43</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="18">
+        <v>44</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="9" t="str">
+        <f>$D$2&amp;"/{0}"</f>
+        <v>/booking/{0}</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="18">
+        <v>45</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="18">
+        <v>46</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="18">
+        <v>47</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" s="9">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="18">
+        <v>48</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
API testcases by creating booking id for valid use cases
</commit_message>
<xml_diff>
--- a/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
+++ b/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Log\GitRepo\internetherokuapp\SourceCode\CSharpSolution\Framework\HerokuAppAutomation\UI.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A457AB46-9DBC-4F1D-A6DF-597CADE69588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2563113-0068-4BF6-B39A-B119BC8CC4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1020,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9087AB3-733F-428C-B4A0-666075F2F7F6}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1308,7 +1308,7 @@
         <v>40</v>
       </c>
       <c r="D20" s="11">
-        <v>1000000</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1606,7 +1606,7 @@
         <v>40</v>
       </c>
       <c r="D42" s="11">
-        <v>1000000</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
API Sample Test Execution Results along with first 5 UI Automation Test cases
</commit_message>
<xml_diff>
--- a/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
+++ b/SourceCode/CSharpSolution/Framework/HerokuAppAutomation/UI.Tests/Data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Log\GitRepo\internetherokuapp\SourceCode\CSharpSolution\Framework\HerokuAppAutomation\UI.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2563113-0068-4BF6-B39A-B119BC8CC4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1C2C0D-EF49-444C-9099-0A433A0AE82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UISuite" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="78">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -298,6 +298,60 @@
   </si>
   <si>
     <t>Test Case 09 - Delete Booking Negative scenario with invalid Booking Id</t>
+  </si>
+  <si>
+    <t>Test Case 4 - Drag And Drop Demonstration</t>
+  </si>
+  <si>
+    <t>Drag and Drop</t>
+  </si>
+  <si>
+    <t>Page Title</t>
+  </si>
+  <si>
+    <t>First Box Title</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Second Box Title</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Test Case 5 - Frames Demonstration</t>
+  </si>
+  <si>
+    <t>Frame Link Text</t>
+  </si>
+  <si>
+    <t>iFrame</t>
+  </si>
+  <si>
+    <t>New Text Message</t>
+  </si>
+  <si>
+    <t>This is an Automated Text written on the iFrame</t>
+  </si>
+  <si>
+    <t>Your content goes here.</t>
+  </si>
+  <si>
+    <t>Default Text Message</t>
+  </si>
+  <si>
+    <t>Test Case 6 - JavaScript Alerts Demonstration</t>
+  </si>
+  <si>
+    <t>Click for JS Confirm</t>
+  </si>
+  <si>
+    <t>You clicked: Cancel</t>
+  </si>
+  <si>
+    <t>Result Text Message</t>
   </si>
 </sst>
 </file>
@@ -388,23 +442,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -734,18 +782,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -756,7 +805,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -764,252 +813,266 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="B13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1020,16 +1083,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9087AB3-733F-428C-B4A0-666075F2F7F6}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" style="20" customWidth="1"/>
-    <col min="2" max="2" width="79.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="18" customWidth="1"/>
+    <col min="2" max="2" width="79.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1040,7 +1104,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1048,661 +1112,661 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="17">
+      <c r="A4" s="15">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="180" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
+      <c r="A5" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="17">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
+      <c r="A7" s="16">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="9" t="str">
+      <c r="D7" s="7" t="str">
         <f>D2</f>
         <v>/booking</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
+      <c r="A8" s="16">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="18">
+      <c r="A9" s="16">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="18">
+      <c r="A10" s="16">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
+      <c r="A11" s="15">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="11" t="str">
+      <c r="D11" s="9" t="str">
         <f>D2</f>
         <v>/booking</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="140.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="17">
+      <c r="A12" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+      <c r="A13" s="15">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="10">
         <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
+      <c r="A14" s="15">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="18">
+      <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="9" t="str">
+      <c r="D15" s="7" t="str">
         <f>$D$2&amp;"/{0}"</f>
         <v>/booking/{0}</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="18">
+      <c r="A16" s="16">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
+      <c r="A17" s="16">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="18">
+      <c r="A18" s="16">
         <v>17</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="17">
+      <c r="A19" s="15">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="11" t="str">
+      <c r="D19" s="9" t="str">
         <f>$D$2&amp;"/{0}"</f>
         <v>/booking/{0}</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="17">
+      <c r="A20" s="15">
         <v>19</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="9">
         <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="17">
+      <c r="A21" s="15">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="9">
         <v>404</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="17">
+      <c r="A22" s="15">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="18">
+      <c r="A23" s="16">
         <v>22</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="9" t="str">
+      <c r="D23" s="7" t="str">
         <f>$D$2&amp;"/{0}"</f>
         <v>/booking/{0}</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="18">
+      <c r="A24" s="16">
         <v>23</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="18">
+      <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="9"/>
+      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="18">
+      <c r="A26" s="16">
         <v>25</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="13" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="18">
+      <c r="A27" s="16">
         <v>26</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="7">
         <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="18">
+      <c r="A28" s="16">
         <v>27</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="17">
+      <c r="A29" s="15">
         <v>28</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="11" t="str">
+      <c r="D29" s="9" t="str">
         <f>$D$2&amp;"/{0}"</f>
         <v>/booking/{0}</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="17">
+      <c r="A30" s="15">
         <v>29</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="11"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="17">
+      <c r="A31" s="15">
         <v>30</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="11"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="141.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="17">
+      <c r="A32" s="15">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="17">
+      <c r="A33" s="15">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="9">
         <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="17">
+      <c r="A34" s="15">
         <v>33</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="18">
+      <c r="A35" s="16">
         <v>34</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="9" t="str">
+      <c r="D35" s="7" t="str">
         <f>$D$2&amp;"/{0}"</f>
         <v>/booking/{0}</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="18">
+      <c r="A36" s="16">
         <v>35</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="9"/>
+      <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="18">
+      <c r="A37" s="16">
         <v>36</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="9"/>
+      <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="18">
+      <c r="A38" s="16">
         <v>37</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="7">
         <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="18">
+      <c r="A39" s="16">
         <v>38</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="17">
+      <c r="A40" s="15">
         <v>39</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="11" t="str">
+      <c r="D40" s="9" t="str">
         <f>$D$2&amp;"/{0}"</f>
         <v>/booking/{0}</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="17">
+      <c r="A41" s="15">
         <v>40</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="11"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="17">
+      <c r="A42" s="15">
         <v>41</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D42" s="9">
         <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="17">
+      <c r="A43" s="15">
         <v>42</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D43" s="9">
         <v>403</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="17">
+      <c r="A44" s="15">
         <v>43</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="17" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="18">
+      <c r="A45" s="16">
         <v>44</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="9" t="str">
+      <c r="D45" s="7" t="str">
         <f>$D$2&amp;"/{0}"</f>
         <v>/booking/{0}</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="18">
+      <c r="A46" s="16">
         <v>45</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="18">
+      <c r="A47" s="16">
         <v>46</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="9"/>
+      <c r="D47" s="7"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="18">
+      <c r="A48" s="16">
         <v>47</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="7">
         <v>403</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="18">
+      <c r="A49" s="16">
         <v>48</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="21" t="s">
+      <c r="D49" s="19" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>